<commit_message>
squash merge of main
</commit_message>
<xml_diff>
--- a/api/source/utils/poam-template.xlsx
+++ b/api/source/utils/poam-template.xlsx
@@ -1,43 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_11C2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gits\github\cd-rite\stig-manager\api\source\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF956613-3CB0-4360-BD11-3BB354BEC4FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5868A7-C32A-4607-9978-4DE8F6C8DF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43335" yWindow="6210" windowWidth="38910" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POA&amp;M" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Control Vulnerability Description</t>
   </si>
   <si>
-    <t>Security Control Number (NC/NA controls only)</t>
-  </si>
-  <si>
     <t>Office/Org</t>
   </si>
   <si>
@@ -50,15 +37,9 @@
     <t>Scheduled Completion Date</t>
   </si>
   <si>
-    <t>Milestone With Completion Dates</t>
-  </si>
-  <si>
     <t>Milestone Changes</t>
   </si>
   <si>
-    <t>Source Identifying Vulnerability</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -71,9 +52,6 @@
     <t>Devices Affected</t>
   </si>
   <si>
-    <t>Mitigations</t>
-  </si>
-  <si>
     <t>Predisposing Conditions</t>
   </si>
   <si>
@@ -86,9 +64,6 @@
     <t>Threat Description</t>
   </si>
   <si>
-    <t>Liklihood</t>
-  </si>
-  <si>
     <t>Impact</t>
   </si>
   <si>
@@ -101,9 +76,6 @@
     <t>Recommendations</t>
   </si>
   <si>
-    <t>Resulting Risk after Proposed Mitigations</t>
-  </si>
-  <si>
     <t>${table:vuln.desc}</t>
   </si>
   <si>
@@ -119,9 +91,6 @@
     <t>${table:vuln.resourcesRequired}</t>
   </si>
   <si>
-    <t>${table:vuln.date}</t>
-  </si>
-  <si>
     <t>${table:vuln.milestone}</t>
   </si>
   <si>
@@ -174,22 +143,38 @@
   </si>
   <si>
     <t>${table:vuln.resultingRisk}</t>
+  </si>
+  <si>
+    <t>POA&amp;M Item ID</t>
+  </si>
+  <si>
+    <t>Controls / APs</t>
+  </si>
+  <si>
+    <t>Milestone ID</t>
+  </si>
+  <si>
+    <t>Milestone with Completion Dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Identifying Vulnerability </t>
+  </si>
+  <si>
+    <t>Mitigations (in-house and in conjunction with the Navy CSSP)</t>
+  </si>
+  <si>
+    <t>Likelihood</t>
+  </si>
+  <si>
+    <t>Resulting Residual Risk after Proposed Mitigations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -203,8 +188,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,7 +210,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0F8FF"/>
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="23"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,27 +250,174 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFBAA77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB1D580"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFBAA77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB1D580"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFBAA77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB1D580"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFBAA77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB1D580"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -543,168 +693,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="24" width="20.7109375" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="24" width="20.7265625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.08984375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="24.453125" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" s="3" customFormat="1" ht="408.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="N1 R1:S1 U1:V1 X1 Z1">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"Very Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Moderate"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>"Very High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="14">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Describe the identified threat(s) and relevance to the information system." sqref="T1" xr:uid="{BFC9D1B9-0F1F-4627-8E9D-5EF12200E6EE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Severity assessment of the relative importance of mitigating/remediating the vulnerability. The severity can be determined by the extent of the potential adverse impact if such a vulnerability is exploited by a threat source." sqref="R1" xr:uid="{B2B7C960-5398-4B89-94EF-3DA940453FD7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Indicate the risk level expected after any proposed mitigations are implemented.  Proposed mitigations should be appropriately documented as POA&amp;M milestones" sqref="Z1" xr:uid="{17D49214-1B2D-4C4D-8212-0861C63C1240}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Determine the relevance of the threat by identifying potential threat events, relevance of the events, and threat sources that could initiate the events" sqref="S1" xr:uid="{D1DE6F9F-B6B8-4B03-B62B-56B75C9CD127}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Provide a summary of the recommended actions that will further address/reduce the risk of this vulnerability." sqref="Y1" xr:uid="{C570944F-3248-4956-A460-EFAF3B41F50A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Identify the initial or starting severity of the vulnerability prior to implementing mitigations and/or compensating Controls. Typically determined by reviewing DISA publication guides, checklists, and/or databases from vulnerability scan engines" sqref="N1" xr:uid="{E8A04826-99EA-4243-B875-D78BB18201C8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="A predisposing condition is a condition existing within an organization, a mission or business process, enterprise architecture, information system/PIT, or environment of operation, which affects liklihood of threat events." sqref="Q1" xr:uid="{767B0414-F09F-4AE9-9752-A54000FED01A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Describe any currently implemented mitigations and/or compensating Controls that will reduce the risk. A planned mitigation or compensating Control cannot lower risk until implemented" sqref="P1" xr:uid="{90CD09FB-3DD7-4F1A-B715-CA43AFCBD7A0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Identify the level of impact as the magnitude of potential harm to organizational operations, organizational assets, individuals, other organizations, or the Nation from the threat event." sqref="V1" xr:uid="{959105AA-E722-45D4-8936-E91E54233B03}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="List any affected devices by hostname. If all devices in the information system are affected, state 'system' or 'all'." sqref="O1" xr:uid="{4D1510B4-A8B3-47DD-82AC-671F2AD69BFC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data:" prompt="Determine the level of risk to organizational operations, organizational assets, individuals, other organizations, or the Nation as a combination of likelihood and impact" sqref="X1" xr:uid="{FDF129B8-F5E9-42C3-8E1B-8247BB881CDB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data:" prompt="Likelihood can be determined as a combination of the vulnerability severity/predisposing condition pervasiveness and the relevance of the threat." sqref="U1" xr:uid="{9DCF5D6A-6559-4BFD-BBD9-8D65F20E2762}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Entry:" prompt="Select appropriate information from the dropdown menu" sqref="L1" xr:uid="{B9786F0F-641B-48D6-AEC8-ECCA555489E4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date Entry:" prompt="MM/DD/YYYY" sqref="G1" xr:uid="{B1A8BF06-82A8-4FE5-8E27-4692CAC1A3DD}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>